<commit_message>
Pie Charts per country, plus rough explantion
I still need to explain the charts, what they represent, and
   the significant differences between countries. BECAUSE FUN.

...I might need to do that. I probably don't need to. But it seems
   like it might be a good idea.
</commit_message>
<xml_diff>
--- a/MechanicalTurkStuff/TranscriptionsPerCountryPieCharts.xlsx
+++ b/MechanicalTurkStuff/TranscriptionsPerCountryPieCharts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="3340" yWindow="40" windowWidth="25600" windowHeight="18460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data Source" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="UniqueTranscribedPhrases">[1]Batch_813445_batch_results.csv!$AL:$AL</definedName>
     <definedName name="WorkerIdValsOnly">[1]Batch_813445_batch_results.csv!$P$2:$P$871</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -10224,11 +10224,12 @@
     <sheetNames>
       <sheetName val="Batch_813445_batch_results.csv"/>
       <sheetName val="rejected HITS"/>
-      <sheetName val="Unique Transcriptions STATIC"/>
       <sheetName val="Unique Transcriptions DYNAMIC"/>
-      <sheetName val="Transcription by country pies"/>
       <sheetName val="All Response Summary charts"/>
       <sheetName val="answer tally vs actualSTATIC"/>
+      <sheetName val="bubble charts"/>
+      <sheetName val="usa Tally vs actualSTATIC"/>
+      <sheetName val="Sheet2"/>
       <sheetName val="answer tally vs wordFreqsCOCA"/>
       <sheetName val="answer tally vs wordFreqsSTATIC"/>
       <sheetName val="india Tally vs actual DYNAMIC"/>
@@ -30399,2469 +30400,7 @@
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="B2" t="str">
-            <v>Worldwide Count</v>
-          </cell>
-          <cell r="C2" t="str">
-            <v>India</v>
-          </cell>
-          <cell r="D2" t="str">
-            <v>Macedonia</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>an ice cold hour</v>
-          </cell>
-          <cell r="B3">
-            <v>370</v>
-          </cell>
-          <cell r="C3">
-            <v>99</v>
-          </cell>
-          <cell r="D3">
-            <v>24</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>a nice cold hour</v>
-          </cell>
-          <cell r="B4">
-            <v>264</v>
-          </cell>
-          <cell r="C4">
-            <v>88</v>
-          </cell>
-          <cell r="D4">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>a nice gold hour</v>
-          </cell>
-          <cell r="B5">
-            <v>63</v>
-          </cell>
-          <cell r="C5">
-            <v>1</v>
-          </cell>
-          <cell r="D5">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>on ice cold hour</v>
-          </cell>
-          <cell r="B6">
-            <v>55</v>
-          </cell>
-          <cell r="C6">
-            <v>9</v>
-          </cell>
-          <cell r="D6">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>in ice cold hour</v>
-          </cell>
-          <cell r="B7">
-            <v>38</v>
-          </cell>
-          <cell r="C7">
-            <v>17</v>
-          </cell>
-          <cell r="D7">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>an ice gold hour</v>
-          </cell>
-          <cell r="B8">
-            <v>18</v>
-          </cell>
-          <cell r="C8">
-            <v>0</v>
-          </cell>
-          <cell r="D8">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>an ice cold grave</v>
-          </cell>
-          <cell r="B9">
-            <v>14</v>
-          </cell>
-          <cell r="C9">
-            <v>14</v>
-          </cell>
-          <cell r="D9">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>an eye scold hour</v>
-          </cell>
-          <cell r="B10">
-            <v>13</v>
-          </cell>
-          <cell r="C10">
-            <v>0</v>
-          </cell>
-          <cell r="D10">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>can i spoke hour</v>
-          </cell>
-          <cell r="B11">
-            <v>12</v>
-          </cell>
-          <cell r="C11">
-            <v>9</v>
-          </cell>
-          <cell r="D11">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>an ice cold dower</v>
-          </cell>
-          <cell r="B12">
-            <v>12</v>
-          </cell>
-          <cell r="C12">
-            <v>0</v>
-          </cell>
-          <cell r="D12">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>a nice old hour</v>
-          </cell>
-          <cell r="B13">
-            <v>10</v>
-          </cell>
-          <cell r="C13">
-            <v>2</v>
-          </cell>
-          <cell r="D13">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>in the ice cold hour</v>
-          </cell>
-          <cell r="B14">
-            <v>9</v>
-          </cell>
-          <cell r="C14">
-            <v>1</v>
-          </cell>
-          <cell r="D14">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>a nice bold hour</v>
-          </cell>
-          <cell r="B15">
-            <v>6</v>
-          </cell>
-          <cell r="C15">
-            <v>0</v>
-          </cell>
-          <cell r="D15">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>an ice coal dower</v>
-          </cell>
-          <cell r="B16">
-            <v>6</v>
-          </cell>
-          <cell r="C16">
-            <v>0</v>
-          </cell>
-          <cell r="D16">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>an ice cold dour</v>
-          </cell>
-          <cell r="B17">
-            <v>5</v>
-          </cell>
-          <cell r="C17">
-            <v>0</v>
-          </cell>
-          <cell r="D17">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>an ice cold bower</v>
-          </cell>
-          <cell r="B18">
-            <v>5</v>
-          </cell>
-          <cell r="C18">
-            <v>1</v>
-          </cell>
-          <cell r="D18">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>a nice gold dollar</v>
-          </cell>
-          <cell r="B19">
-            <v>4</v>
-          </cell>
-          <cell r="C19">
-            <v>2</v>
-          </cell>
-          <cell r="D19">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20" t="str">
-            <v>a nine scold hour</v>
-          </cell>
-          <cell r="B20">
-            <v>4</v>
-          </cell>
-          <cell r="C20">
-            <v>0</v>
-          </cell>
-          <cell r="D20">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21" t="str">
-            <v>and i scold hour</v>
-          </cell>
-          <cell r="B21">
-            <v>4</v>
-          </cell>
-          <cell r="C21">
-            <v>0</v>
-          </cell>
-          <cell r="D21">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22" t="str">
-            <v>an ice cold our</v>
-          </cell>
-          <cell r="B22">
-            <v>4</v>
-          </cell>
-          <cell r="C22">
-            <v>2</v>
-          </cell>
-          <cell r="D22">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23" t="str">
-            <v>an iced cold hour</v>
-          </cell>
-          <cell r="B23">
-            <v>4</v>
-          </cell>
-          <cell r="C23">
-            <v>0</v>
-          </cell>
-          <cell r="D23">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24" t="str">
-            <v>an nice cold hour</v>
-          </cell>
-          <cell r="B24">
-            <v>4</v>
-          </cell>
-          <cell r="C24">
-            <v>0</v>
-          </cell>
-          <cell r="D24">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25" t="str">
-            <v>all ice cold hour</v>
-          </cell>
-          <cell r="B25">
-            <v>4</v>
-          </cell>
-          <cell r="C25">
-            <v>0</v>
-          </cell>
-          <cell r="D25">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26" t="str">
-            <v>a nice screwdriver</v>
-          </cell>
-          <cell r="B26">
-            <v>3</v>
-          </cell>
-          <cell r="C26">
-            <v>3</v>
-          </cell>
-          <cell r="D26">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27" t="str">
-            <v>a nights cold hour</v>
-          </cell>
-          <cell r="B27">
-            <v>3</v>
-          </cell>
-          <cell r="C27">
-            <v>0</v>
-          </cell>
-          <cell r="D27">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28" t="str">
-            <v>a nice cold dour</v>
-          </cell>
-          <cell r="B28">
-            <v>3</v>
-          </cell>
-          <cell r="C28">
-            <v>0</v>
-          </cell>
-          <cell r="D28">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29" t="str">
-            <v>ei nice cold hour</v>
-          </cell>
-          <cell r="B29">
-            <v>3</v>
-          </cell>
-          <cell r="C29">
-            <v>0</v>
-          </cell>
-          <cell r="D29">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30" t="str">
-            <v>a nice spoke hour</v>
-          </cell>
-          <cell r="B30">
-            <v>3</v>
-          </cell>
-          <cell r="C30">
-            <v>2</v>
-          </cell>
-          <cell r="D30">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31" t="str">
-            <v>a nice scold hour</v>
-          </cell>
-          <cell r="B31">
-            <v>3</v>
-          </cell>
-          <cell r="C31">
-            <v>0</v>
-          </cell>
-          <cell r="D31">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32" t="str">
-            <v>a nice cold our</v>
-          </cell>
-          <cell r="B32">
-            <v>3</v>
-          </cell>
-          <cell r="C32">
-            <v>1</v>
-          </cell>
-          <cell r="D32">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33" t="str">
-            <v>and i scold our</v>
-          </cell>
-          <cell r="B33">
-            <v>3</v>
-          </cell>
-          <cell r="C33">
-            <v>0</v>
-          </cell>
-          <cell r="D33">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34" t="str">
-            <v>an ice coal dour</v>
-          </cell>
-          <cell r="B34">
-            <v>3</v>
-          </cell>
-          <cell r="C34">
-            <v>0</v>
-          </cell>
-          <cell r="D34">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35" t="str">
-            <v>in ice coal dour</v>
-          </cell>
-          <cell r="B35">
-            <v>3</v>
-          </cell>
-          <cell r="C35">
-            <v>0</v>
-          </cell>
-          <cell r="D35">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36" t="str">
-            <v>an ice core bower</v>
-          </cell>
-          <cell r="B36">
-            <v>3</v>
-          </cell>
-          <cell r="C36">
-            <v>3</v>
-          </cell>
-          <cell r="D36">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37" t="str">
-            <v>on ice cold dower</v>
-          </cell>
-          <cell r="B37">
-            <v>3</v>
-          </cell>
-          <cell r="C37">
-            <v>0</v>
-          </cell>
-          <cell r="D37">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38" t="str">
-            <v>hey nice go the our</v>
-          </cell>
-          <cell r="B38">
-            <v>2</v>
-          </cell>
-          <cell r="C38">
-            <v>0</v>
-          </cell>
-          <cell r="D38">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39" t="str">
-            <v>a nice coal dower</v>
-          </cell>
-          <cell r="B39">
-            <v>2</v>
-          </cell>
-          <cell r="C39">
-            <v>0</v>
-          </cell>
-          <cell r="D39">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40" t="str">
-            <v>a nice cob bower</v>
-          </cell>
-          <cell r="B40">
-            <v>2</v>
-          </cell>
-          <cell r="C40">
-            <v>2</v>
-          </cell>
-          <cell r="D40">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41" t="str">
-            <v>the nice cold hour</v>
-          </cell>
-          <cell r="B41">
-            <v>2</v>
-          </cell>
-          <cell r="C41">
-            <v>1</v>
-          </cell>
-          <cell r="D41">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42" t="str">
-            <v>hey nice go there where</v>
-          </cell>
-          <cell r="B42">
-            <v>2</v>
-          </cell>
-          <cell r="C42">
-            <v>0</v>
-          </cell>
-          <cell r="D42">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="A43" t="str">
-            <v>a nigh scold hour</v>
-          </cell>
-          <cell r="B43">
-            <v>2</v>
-          </cell>
-          <cell r="C43">
-            <v>0</v>
-          </cell>
-          <cell r="D43">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="A44" t="str">
-            <v>a nice gold dower</v>
-          </cell>
-          <cell r="B44">
-            <v>2</v>
-          </cell>
-          <cell r="C44">
-            <v>0</v>
-          </cell>
-          <cell r="D44">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="A45" t="str">
-            <v>hey nice screwdriver</v>
-          </cell>
-          <cell r="B45">
-            <v>2</v>
-          </cell>
-          <cell r="C45">
-            <v>2</v>
-          </cell>
-          <cell r="D45">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="A46" t="str">
-            <v>a nice fold hour</v>
-          </cell>
-          <cell r="B46">
-            <v>2</v>
-          </cell>
-          <cell r="C46">
-            <v>0</v>
-          </cell>
-          <cell r="D46">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="A47" t="str">
-            <v>an ice old hour</v>
-          </cell>
-          <cell r="B47">
-            <v>2</v>
-          </cell>
-          <cell r="C47">
-            <v>0</v>
-          </cell>
-          <cell r="D47">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="A48" t="str">
-            <v>an ice scold hour</v>
-          </cell>
-          <cell r="B48">
-            <v>2</v>
-          </cell>
-          <cell r="C48">
-            <v>0</v>
-          </cell>
-          <cell r="D48">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="A49" t="str">
-            <v>in i scold hour</v>
-          </cell>
-          <cell r="B49">
-            <v>2</v>
-          </cell>
-          <cell r="C49">
-            <v>0</v>
-          </cell>
-          <cell r="D49">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="A50" t="str">
-            <v>n i screwdriver</v>
-          </cell>
-          <cell r="B50">
-            <v>2</v>
-          </cell>
-          <cell r="C50">
-            <v>2</v>
-          </cell>
-          <cell r="D50">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="A51" t="str">
-            <v>an i scold hour</v>
-          </cell>
-          <cell r="B51">
-            <v>2</v>
-          </cell>
-          <cell r="C51">
-            <v>0</v>
-          </cell>
-          <cell r="D51">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="A52" t="str">
-            <v>on ice coal dour</v>
-          </cell>
-          <cell r="B52">
-            <v>2</v>
-          </cell>
-          <cell r="C52">
-            <v>0</v>
-          </cell>
-          <cell r="D52">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="A53" t="str">
-            <v>an ice cold shower</v>
-          </cell>
-          <cell r="B53">
-            <v>2</v>
-          </cell>
-          <cell r="C53">
-            <v>0</v>
-          </cell>
-          <cell r="D53">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="A54" t="str">
-            <v>an i screwdriver</v>
-          </cell>
-          <cell r="B54">
-            <v>2</v>
-          </cell>
-          <cell r="C54">
-            <v>2</v>
-          </cell>
-          <cell r="D54">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="A55" t="str">
-            <v>in ice cold davar</v>
-          </cell>
-          <cell r="B55">
-            <v>2</v>
-          </cell>
-          <cell r="C55">
-            <v>2</v>
-          </cell>
-          <cell r="D55">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="A56" t="str">
-            <v>an ice cole dower</v>
-          </cell>
-          <cell r="B56">
-            <v>2</v>
-          </cell>
-          <cell r="C56">
-            <v>2</v>
-          </cell>
-          <cell r="D56">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="A57" t="str">
-            <v>an eyes close over</v>
-          </cell>
-          <cell r="B57">
-            <v>2</v>
-          </cell>
-          <cell r="C57">
-            <v>2</v>
-          </cell>
-          <cell r="D57">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="A58" t="str">
-            <v>an ice-cold hour</v>
-          </cell>
-          <cell r="B58">
-            <v>2</v>
-          </cell>
-          <cell r="C58">
-            <v>1</v>
-          </cell>
-          <cell r="D58">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="59">
-          <cell r="A59" t="str">
-            <v>an ice cold dollar</v>
-          </cell>
-          <cell r="B59">
-            <v>2</v>
-          </cell>
-          <cell r="C59">
-            <v>0</v>
-          </cell>
-          <cell r="D59">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="A60" t="str">
-            <v>in unschooled hour</v>
-          </cell>
-          <cell r="B60">
-            <v>2</v>
-          </cell>
-          <cell r="C60">
-            <v>0</v>
-          </cell>
-          <cell r="D60">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="A61" t="str">
-            <v>in nice cold hour</v>
-          </cell>
-          <cell r="B61">
-            <v>2</v>
-          </cell>
-          <cell r="C61">
-            <v>0</v>
-          </cell>
-          <cell r="D61">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="A62" t="str">
-            <v>and nice cold hour</v>
-          </cell>
-          <cell r="B62">
-            <v>2</v>
-          </cell>
-          <cell r="C62">
-            <v>0</v>
-          </cell>
-          <cell r="D62">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="A63" t="str">
-            <v>a nice cool dower</v>
-          </cell>
-          <cell r="B63">
-            <v>1</v>
-          </cell>
-          <cell r="C63">
-            <v>0</v>
-          </cell>
-          <cell r="D63">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="A64" t="str">
-            <v>a nice cold thou are</v>
-          </cell>
-          <cell r="B64">
-            <v>1</v>
-          </cell>
-          <cell r="C64">
-            <v>0</v>
-          </cell>
-          <cell r="D64">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="A65" t="str">
-            <v>a nice coal dour</v>
-          </cell>
-          <cell r="B65">
-            <v>1</v>
-          </cell>
-          <cell r="C65">
-            <v>0</v>
-          </cell>
-          <cell r="D65">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="A66" t="str">
-            <v>a nice cow is there</v>
-          </cell>
-          <cell r="B66">
-            <v>1</v>
-          </cell>
-          <cell r="C66">
-            <v>1</v>
-          </cell>
-          <cell r="D66">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="A67" t="str">
-            <v>enoise cothawer</v>
-          </cell>
-          <cell r="B67">
-            <v>1</v>
-          </cell>
-          <cell r="C67">
-            <v>1</v>
-          </cell>
-          <cell r="D67">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="A68" t="str">
-            <v>nice cold hour</v>
-          </cell>
-          <cell r="B68">
-            <v>1</v>
-          </cell>
-          <cell r="C68">
-            <v>1</v>
-          </cell>
-          <cell r="D68">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="A69" t="str">
-            <v>a nice could hour</v>
-          </cell>
-          <cell r="B69">
-            <v>1</v>
-          </cell>
-          <cell r="C69">
-            <v>0</v>
-          </cell>
-          <cell r="D69">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="A70" t="str">
-            <v>an ice hold power</v>
-          </cell>
-          <cell r="B70">
-            <v>1</v>
-          </cell>
-          <cell r="C70">
-            <v>1</v>
-          </cell>
-          <cell r="D70">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="71">
-          <cell r="A71" t="str">
-            <v>a nice screw driver</v>
-          </cell>
-          <cell r="B71">
-            <v>1</v>
-          </cell>
-          <cell r="C71">
-            <v>1</v>
-          </cell>
-          <cell r="D71">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="A72" t="str">
-            <v>a nice cob our</v>
-          </cell>
-          <cell r="B72">
-            <v>1</v>
-          </cell>
-          <cell r="C72">
-            <v>1</v>
-          </cell>
-          <cell r="D72">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="A73" t="str">
-            <v>a nice scold dower</v>
-          </cell>
-          <cell r="B73">
-            <v>1</v>
-          </cell>
-          <cell r="C73">
-            <v>0</v>
-          </cell>
-          <cell r="D73">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="A74" t="str">
-            <v>a nine skulled hour</v>
-          </cell>
-          <cell r="B74">
-            <v>1</v>
-          </cell>
-          <cell r="C74">
-            <v>0</v>
-          </cell>
-          <cell r="D74">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="A75" t="str">
-            <v>ah nay skull dower</v>
-          </cell>
-          <cell r="B75">
-            <v>1</v>
-          </cell>
-          <cell r="C75">
-            <v>0</v>
-          </cell>
-          <cell r="D75">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="A76" t="str">
-            <v>a nice scored hour</v>
-          </cell>
-          <cell r="B76">
-            <v>1</v>
-          </cell>
-          <cell r="C76">
-            <v>1</v>
-          </cell>
-          <cell r="D76">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="77">
-          <cell r="A77" t="str">
-            <v>a nye scoldower</v>
-          </cell>
-          <cell r="B77">
-            <v>1</v>
-          </cell>
-          <cell r="C77">
-            <v>0</v>
-          </cell>
-          <cell r="D77">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="78">
-          <cell r="A78" t="str">
-            <v>hey nine scold hour</v>
-          </cell>
-          <cell r="B78">
-            <v>1</v>
-          </cell>
-          <cell r="C78">
-            <v>0</v>
-          </cell>
-          <cell r="D78">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="A79" t="str">
-            <v>a nice called hour</v>
-          </cell>
-          <cell r="B79">
-            <v>1</v>
-          </cell>
-          <cell r="C79">
-            <v>1</v>
-          </cell>
-          <cell r="D79">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="A80" t="str">
-            <v>a nice cold bowl</v>
-          </cell>
-          <cell r="B80">
-            <v>1</v>
-          </cell>
-          <cell r="C80">
-            <v>1</v>
-          </cell>
-          <cell r="D80">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="A81" t="str">
-            <v>a nice cold dollar</v>
-          </cell>
-          <cell r="B81">
-            <v>1</v>
-          </cell>
-          <cell r="C81">
-            <v>1</v>
-          </cell>
-          <cell r="D81">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="A82" t="str">
-            <v>a nice for the hour</v>
-          </cell>
-          <cell r="B82">
-            <v>1</v>
-          </cell>
-          <cell r="C82">
-            <v>1</v>
-          </cell>
-          <cell r="D82">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="A83" t="str">
-            <v>in ice old hour</v>
-          </cell>
-          <cell r="B83">
-            <v>1</v>
-          </cell>
-          <cell r="C83">
-            <v>1</v>
-          </cell>
-          <cell r="D83">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="84">
-          <cell r="A84" t="str">
-            <v>a nice odd hour</v>
-          </cell>
-          <cell r="B84">
-            <v>1</v>
-          </cell>
-          <cell r="C84">
-            <v>1</v>
-          </cell>
-          <cell r="D84">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="A85" t="str">
-            <v>a nice pod our</v>
-          </cell>
-          <cell r="B85">
-            <v>1</v>
-          </cell>
-          <cell r="C85">
-            <v>1</v>
-          </cell>
-          <cell r="D85">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="A86" t="str">
-            <v>a nice code hour</v>
-          </cell>
-          <cell r="B86">
-            <v>1</v>
-          </cell>
-          <cell r="C86">
-            <v>1</v>
-          </cell>
-          <cell r="D86">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="A87" t="str">
-            <v>ej nice cold ohur</v>
-          </cell>
-          <cell r="B87">
-            <v>1</v>
-          </cell>
-          <cell r="C87">
-            <v>0</v>
-          </cell>
-          <cell r="D87">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="A88" t="str">
-            <v>hey nice hold hour</v>
-          </cell>
-          <cell r="B88">
-            <v>1</v>
-          </cell>
-          <cell r="C88">
-            <v>0</v>
-          </cell>
-          <cell r="D88">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="A89" t="str">
-            <v>a nice school bower</v>
-          </cell>
-          <cell r="B89">
-            <v>1</v>
-          </cell>
-          <cell r="C89">
-            <v>1</v>
-          </cell>
-          <cell r="D89">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="90">
-          <cell r="A90" t="str">
-            <v>a nice godfather</v>
-          </cell>
-          <cell r="B90">
-            <v>1</v>
-          </cell>
-          <cell r="C90">
-            <v>1</v>
-          </cell>
-          <cell r="D90">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="A91" t="str">
-            <v>ej nice cold hout</v>
-          </cell>
-          <cell r="B91">
-            <v>1</v>
-          </cell>
-          <cell r="C91">
-            <v>0</v>
-          </cell>
-          <cell r="D91">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="A92" t="str">
-            <v>a nine spole dower</v>
-          </cell>
-          <cell r="B92">
-            <v>1</v>
-          </cell>
-          <cell r="C92">
-            <v>0</v>
-          </cell>
-          <cell r="D92">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="A93" t="str">
-            <v>a nice cobour</v>
-          </cell>
-          <cell r="B93">
-            <v>1</v>
-          </cell>
-          <cell r="C93">
-            <v>1</v>
-          </cell>
-          <cell r="D93">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="A94" t="str">
-            <v>he nice on the hour</v>
-          </cell>
-          <cell r="B94">
-            <v>1</v>
-          </cell>
-          <cell r="C94">
-            <v>1</v>
-          </cell>
-          <cell r="D94">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="A95" t="str">
-            <v>a nice gold dour</v>
-          </cell>
-          <cell r="B95">
-            <v>1</v>
-          </cell>
-          <cell r="C95">
-            <v>0</v>
-          </cell>
-          <cell r="D95">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="96">
-          <cell r="A96" t="str">
-            <v>an i scold dour</v>
-          </cell>
-          <cell r="B96">
-            <v>1</v>
-          </cell>
-          <cell r="C96">
-            <v>0</v>
-          </cell>
-          <cell r="D96">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="A97" t="str">
-            <v>an eye scold our</v>
-          </cell>
-          <cell r="B97">
-            <v>1</v>
-          </cell>
-          <cell r="C97">
-            <v>0</v>
-          </cell>
-          <cell r="D97">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="A98" t="str">
-            <v>an eye scol dagr</v>
-          </cell>
-          <cell r="B98">
-            <v>1</v>
-          </cell>
-          <cell r="C98">
-            <v>0</v>
-          </cell>
-          <cell r="D98">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="A99" t="str">
-            <v>an ice bore bower</v>
-          </cell>
-          <cell r="B99">
-            <v>1</v>
-          </cell>
-          <cell r="C99">
-            <v>1</v>
-          </cell>
-          <cell r="D99">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="A100" t="str">
-            <v>an ice gold dower</v>
-          </cell>
-          <cell r="B100">
-            <v>1</v>
-          </cell>
-          <cell r="C100">
-            <v>0</v>
-          </cell>
-          <cell r="D100">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="A101" t="str">
-            <v>hen ice oh dawad</v>
-          </cell>
-          <cell r="B101">
-            <v>1</v>
-          </cell>
-          <cell r="C101">
-            <v>1</v>
-          </cell>
-          <cell r="D101">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="102">
-          <cell r="A102" t="str">
-            <v>in eye spole dower</v>
-          </cell>
-          <cell r="B102">
-            <v>1</v>
-          </cell>
-          <cell r="C102">
-            <v>0</v>
-          </cell>
-          <cell r="D102">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="103">
-          <cell r="A103" t="str">
-            <v>and i scored over</v>
-          </cell>
-          <cell r="B103">
-            <v>1</v>
-          </cell>
-          <cell r="C103">
-            <v>1</v>
-          </cell>
-          <cell r="D103">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="104">
-          <cell r="A104" t="str">
-            <v>a nice cold shower</v>
-          </cell>
-          <cell r="B104">
-            <v>1</v>
-          </cell>
-          <cell r="C104">
-            <v>0</v>
-          </cell>
-          <cell r="D104">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="105">
-          <cell r="A105" t="str">
-            <v>an ounce gold hour</v>
-          </cell>
-          <cell r="B105">
-            <v>1</v>
-          </cell>
-          <cell r="C105">
-            <v>0</v>
-          </cell>
-          <cell r="D105">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="106">
-          <cell r="A106" t="str">
-            <v>an eyes cold hour</v>
-          </cell>
-          <cell r="B106">
-            <v>1</v>
-          </cell>
-          <cell r="C106">
-            <v>0</v>
-          </cell>
-          <cell r="D106">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="107">
-          <cell r="A107" t="str">
-            <v>an ice hold hour</v>
-          </cell>
-          <cell r="B107">
-            <v>1</v>
-          </cell>
-          <cell r="C107">
-            <v>0</v>
-          </cell>
-          <cell r="D107">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="108">
-          <cell r="A108" t="str">
-            <v>and i scored the hour</v>
-          </cell>
-          <cell r="B108">
-            <v>1</v>
-          </cell>
-          <cell r="C108">
-            <v>1</v>
-          </cell>
-          <cell r="D108">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="109">
-          <cell r="A109" t="str">
-            <v>an ice cold ower</v>
-          </cell>
-          <cell r="B109">
-            <v>1</v>
-          </cell>
-          <cell r="C109">
-            <v>0</v>
-          </cell>
-          <cell r="D109">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="110">
-          <cell r="A110" t="str">
-            <v>an ice cob our</v>
-          </cell>
-          <cell r="B110">
-            <v>1</v>
-          </cell>
-          <cell r="C110">
-            <v>1</v>
-          </cell>
-          <cell r="D110">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="A111" t="str">
-            <v>in nice code over</v>
-          </cell>
-          <cell r="B111">
-            <v>1</v>
-          </cell>
-          <cell r="C111">
-            <v>1</v>
-          </cell>
-          <cell r="D111">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="112">
-          <cell r="A112" t="str">
-            <v>an eyes co thou</v>
-          </cell>
-          <cell r="B112">
-            <v>1</v>
-          </cell>
-          <cell r="C112">
-            <v>1</v>
-          </cell>
-          <cell r="D112">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="113">
-          <cell r="A113" t="str">
-            <v>in ice cold dour</v>
-          </cell>
-          <cell r="B113">
-            <v>1</v>
-          </cell>
-          <cell r="C113">
-            <v>0</v>
-          </cell>
-          <cell r="D113">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="114">
-          <cell r="A114" t="str">
-            <v>and ice cold dollar</v>
-          </cell>
-          <cell r="B114">
-            <v>1</v>
-          </cell>
-          <cell r="C114">
-            <v>0</v>
-          </cell>
-          <cell r="D114">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="115">
-          <cell r="A115" t="str">
-            <v>an ice cold bowl</v>
-          </cell>
-          <cell r="B115">
-            <v>1</v>
-          </cell>
-          <cell r="C115">
-            <v>1</v>
-          </cell>
-          <cell r="D115">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="116">
-          <cell r="A116" t="str">
-            <v>i saw tower</v>
-          </cell>
-          <cell r="B116">
-            <v>1</v>
-          </cell>
-          <cell r="C116">
-            <v>1</v>
-          </cell>
-          <cell r="D116">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="117">
-          <cell r="A117" t="str">
-            <v>in icecube daver</v>
-          </cell>
-          <cell r="B117">
-            <v>1</v>
-          </cell>
-          <cell r="C117">
-            <v>1</v>
-          </cell>
-          <cell r="D117">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="118">
-          <cell r="A118" t="str">
-            <v>in ice gold hour</v>
-          </cell>
-          <cell r="B118">
-            <v>1</v>
-          </cell>
-          <cell r="C118">
-            <v>0</v>
-          </cell>
-          <cell r="D118">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="119">
-          <cell r="A119" t="str">
-            <v>then ices co the where</v>
-          </cell>
-          <cell r="B119">
-            <v>1</v>
-          </cell>
-          <cell r="C119">
-            <v>0</v>
-          </cell>
-          <cell r="D119">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="120">
-          <cell r="A120" t="str">
-            <v>ni screwdriver</v>
-          </cell>
-          <cell r="B120">
-            <v>1</v>
-          </cell>
-          <cell r="C120">
-            <v>1</v>
-          </cell>
-          <cell r="D120">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="121">
-          <cell r="A121" t="str">
-            <v>a nice cool hour</v>
-          </cell>
-          <cell r="B121">
-            <v>1</v>
-          </cell>
-          <cell r="C121">
-            <v>1</v>
-          </cell>
-          <cell r="D121">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="122">
-          <cell r="A122" t="str">
-            <v>can i score the hour</v>
-          </cell>
-          <cell r="B122">
-            <v>1</v>
-          </cell>
-          <cell r="C122">
-            <v>1</v>
-          </cell>
-          <cell r="D122">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="123">
-          <cell r="A123" t="str">
-            <v>in nice code our</v>
-          </cell>
-          <cell r="B123">
-            <v>1</v>
-          </cell>
-          <cell r="C123">
-            <v>1</v>
-          </cell>
-          <cell r="D123">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="124">
-          <cell r="A124" t="str">
-            <v>an ice cool bower</v>
-          </cell>
-          <cell r="B124">
-            <v>1</v>
-          </cell>
-          <cell r="C124">
-            <v>0</v>
-          </cell>
-          <cell r="D124">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="125">
-          <cell r="A125" t="str">
-            <v>then ice hole power</v>
-          </cell>
-          <cell r="B125">
-            <v>1</v>
-          </cell>
-          <cell r="C125">
-            <v>1</v>
-          </cell>
-          <cell r="D125">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="126">
-          <cell r="A126" t="str">
-            <v>an i screw driver</v>
-          </cell>
-          <cell r="B126">
-            <v>1</v>
-          </cell>
-          <cell r="C126">
-            <v>1</v>
-          </cell>
-          <cell r="D126">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="127">
-          <cell r="A127" t="str">
-            <v>in ice co daver</v>
-          </cell>
-          <cell r="B127">
-            <v>1</v>
-          </cell>
-          <cell r="C127">
-            <v>1</v>
-          </cell>
-          <cell r="D127">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="128">
-          <cell r="A128" t="str">
-            <v>in ice-cold hour</v>
-          </cell>
-          <cell r="B128">
-            <v>1</v>
-          </cell>
-          <cell r="C128">
-            <v>0</v>
-          </cell>
-          <cell r="D128">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="129">
-          <cell r="A129" t="str">
-            <v>an iced cold dower</v>
-          </cell>
-          <cell r="B129">
-            <v>1</v>
-          </cell>
-          <cell r="C129">
-            <v>0</v>
-          </cell>
-          <cell r="D129">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="130">
-          <cell r="A130" t="str">
-            <v>an ice called dower</v>
-          </cell>
-          <cell r="B130">
-            <v>1</v>
-          </cell>
-          <cell r="C130">
-            <v>1</v>
-          </cell>
-          <cell r="D130">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="131">
-          <cell r="A131" t="str">
-            <v>an ice cove daver</v>
-          </cell>
-          <cell r="B131">
-            <v>1</v>
-          </cell>
-          <cell r="C131">
-            <v>1</v>
-          </cell>
-          <cell r="D131">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="132">
-          <cell r="A132" t="str">
-            <v>then ice go their were</v>
-          </cell>
-          <cell r="B132">
-            <v>1</v>
-          </cell>
-          <cell r="C132">
-            <v>0</v>
-          </cell>
-          <cell r="D132">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="133">
-          <cell r="A133" t="str">
-            <v>hen eyes oh dawad</v>
-          </cell>
-          <cell r="B133">
-            <v>1</v>
-          </cell>
-          <cell r="C133">
-            <v>1</v>
-          </cell>
-          <cell r="D133">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="134">
-          <cell r="A134" t="str">
-            <v>an ice cold bauer</v>
-          </cell>
-          <cell r="B134">
-            <v>1</v>
-          </cell>
-          <cell r="C134">
-            <v>0</v>
-          </cell>
-          <cell r="D134">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="135">
-          <cell r="A135" t="str">
-            <v>then ice go there  our</v>
-          </cell>
-          <cell r="B135">
-            <v>1</v>
-          </cell>
-          <cell r="C135">
-            <v>0</v>
-          </cell>
-          <cell r="D135">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="136">
-          <cell r="A136" t="str">
-            <v>in a ice cool hour</v>
-          </cell>
-          <cell r="B136">
-            <v>1</v>
-          </cell>
-          <cell r="C136">
-            <v>1</v>
-          </cell>
-          <cell r="D136">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="137">
-          <cell r="A137" t="str">
-            <v>in the eyeschool tower</v>
-          </cell>
-          <cell r="B137">
-            <v>1</v>
-          </cell>
-          <cell r="C137">
-            <v>0</v>
-          </cell>
-          <cell r="D137">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="138">
-          <cell r="A138" t="str">
-            <v>in ice called our</v>
-          </cell>
-          <cell r="B138">
-            <v>1</v>
-          </cell>
-          <cell r="C138">
-            <v>0</v>
-          </cell>
-          <cell r="D138">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="139">
-          <cell r="A139" t="str">
-            <v>in a ice cold hour</v>
-          </cell>
-          <cell r="B139">
-            <v>1</v>
-          </cell>
-          <cell r="C139">
-            <v>1</v>
-          </cell>
-          <cell r="D139">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="140">
-          <cell r="A140" t="str">
-            <v>in ice code our</v>
-          </cell>
-          <cell r="B140">
-            <v>1</v>
-          </cell>
-          <cell r="C140">
-            <v>1</v>
-          </cell>
-          <cell r="D140">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="141">
-          <cell r="A141" t="str">
-            <v>an ice could hour</v>
-          </cell>
-          <cell r="B141">
-            <v>1</v>
-          </cell>
-          <cell r="C141">
-            <v>0</v>
-          </cell>
-          <cell r="D141">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="142">
-          <cell r="A142" t="str">
-            <v>hen eyes oh gawd</v>
-          </cell>
-          <cell r="B142">
-            <v>1</v>
-          </cell>
-          <cell r="C142">
-            <v>1</v>
-          </cell>
-          <cell r="D142">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="143">
-          <cell r="A143" t="str">
-            <v>an ice go the our</v>
-          </cell>
-          <cell r="B143">
-            <v>1</v>
-          </cell>
-          <cell r="C143">
-            <v>0</v>
-          </cell>
-          <cell r="D143">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="144">
-          <cell r="A144" t="str">
-            <v>in high school hour</v>
-          </cell>
-          <cell r="B144">
-            <v>1</v>
-          </cell>
-          <cell r="C144">
-            <v>1</v>
-          </cell>
-          <cell r="D144">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="145">
-          <cell r="A145" t="str">
-            <v>a nice cool dollar</v>
-          </cell>
-          <cell r="B145">
-            <v>1</v>
-          </cell>
-          <cell r="C145">
-            <v>1</v>
-          </cell>
-          <cell r="D145">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="146">
-          <cell r="A146" t="str">
-            <v>in ice cold our</v>
-          </cell>
-          <cell r="B146">
-            <v>1</v>
-          </cell>
-          <cell r="C146">
-            <v>0</v>
-          </cell>
-          <cell r="D146">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="147">
-          <cell r="A147" t="str">
-            <v>an ice cold thou are</v>
-          </cell>
-          <cell r="B147">
-            <v>1</v>
-          </cell>
-          <cell r="C147">
-            <v>0</v>
-          </cell>
-          <cell r="D147">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="148">
-          <cell r="A148" t="str">
-            <v>an nice cold our</v>
-          </cell>
-          <cell r="B148">
-            <v>1</v>
-          </cell>
-          <cell r="C148">
-            <v>0</v>
-          </cell>
-          <cell r="D148">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="149">
-          <cell r="A149" t="str">
-            <v>in eyes cold over</v>
-          </cell>
-          <cell r="B149">
-            <v>1</v>
-          </cell>
-          <cell r="C149">
-            <v>1</v>
-          </cell>
-          <cell r="D149">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="150">
-          <cell r="A150" t="str">
-            <v>a nice cold hout</v>
-          </cell>
-          <cell r="B150">
-            <v>1</v>
-          </cell>
-          <cell r="C150">
-            <v>1</v>
-          </cell>
-          <cell r="D150">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="151">
-          <cell r="A151" t="str">
-            <v>a nice go the our</v>
-          </cell>
-          <cell r="B151">
-            <v>1</v>
-          </cell>
-          <cell r="C151">
-            <v>0</v>
-          </cell>
-          <cell r="D151">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="152">
-          <cell r="A152" t="str">
-            <v>a nice cool bowl</v>
-          </cell>
-          <cell r="B152">
-            <v>1</v>
-          </cell>
-          <cell r="C152">
-            <v>1</v>
-          </cell>
-          <cell r="D152">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="153">
-          <cell r="A153" t="str">
-            <v>a light cold hour</v>
-          </cell>
-          <cell r="B153">
-            <v>1</v>
-          </cell>
-          <cell r="C153">
-            <v>0</v>
-          </cell>
-          <cell r="D153">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="154">
-          <cell r="A154" t="str">
-            <v>a niceco daver</v>
-          </cell>
-          <cell r="B154">
-            <v>1</v>
-          </cell>
-          <cell r="C154">
-            <v>1</v>
-          </cell>
-          <cell r="D154">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="155">
-          <cell r="A155" t="str">
-            <v>a nice cold dower</v>
-          </cell>
-          <cell r="B155">
-            <v>1</v>
-          </cell>
-          <cell r="C155">
-            <v>0</v>
-          </cell>
-          <cell r="D155">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="156">
-          <cell r="A156" t="str">
-            <v>an eyes hold power</v>
-          </cell>
-          <cell r="B156">
-            <v>1</v>
-          </cell>
-          <cell r="C156">
-            <v>1</v>
-          </cell>
-          <cell r="D156">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="157">
-          <cell r="A157" t="str">
-            <v>on i screwdriver</v>
-          </cell>
-          <cell r="B157">
-            <v>1</v>
-          </cell>
-          <cell r="C157">
-            <v>1</v>
-          </cell>
-          <cell r="D157">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="158">
-          <cell r="A158" t="str">
-            <v>on ice old hour</v>
-          </cell>
-          <cell r="B158">
-            <v>1</v>
-          </cell>
-          <cell r="C158">
-            <v>0</v>
-          </cell>
-          <cell r="D158">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="159">
-          <cell r="A159" t="str">
-            <v>on the ice cold hour</v>
-          </cell>
-          <cell r="B159">
-            <v>1</v>
-          </cell>
-          <cell r="C159">
-            <v>0</v>
-          </cell>
-          <cell r="D159">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="160">
-          <cell r="A160" t="str">
-            <v>on the ice cold dour</v>
-          </cell>
-          <cell r="B160">
-            <v>1</v>
-          </cell>
-          <cell r="C160">
-            <v>0</v>
-          </cell>
-          <cell r="D160">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="161">
-          <cell r="A161" t="str">
-            <v>on ice cold thou art</v>
-          </cell>
-          <cell r="B161">
-            <v>1</v>
-          </cell>
-          <cell r="C161">
-            <v>0</v>
-          </cell>
-          <cell r="D161">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="162">
-          <cell r="A162" t="str">
-            <v>on ice called our</v>
-          </cell>
-          <cell r="B162">
-            <v>1</v>
-          </cell>
-          <cell r="C162">
-            <v>0</v>
-          </cell>
-          <cell r="D162">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="163">
-          <cell r="A163" t="str">
-            <v>on ice col dour</v>
-          </cell>
-          <cell r="B163">
-            <v>1</v>
-          </cell>
-          <cell r="C163">
-            <v>0</v>
-          </cell>
-          <cell r="D163">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="164">
-          <cell r="A164" t="str">
-            <v>on ice cold bauer</v>
-          </cell>
-          <cell r="B164">
-            <v>1</v>
-          </cell>
-          <cell r="C164">
-            <v>0</v>
-          </cell>
-          <cell r="D164">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="165">
-          <cell r="A165" t="str">
-            <v>on eyes go there</v>
-          </cell>
-          <cell r="B165">
-            <v>1</v>
-          </cell>
-          <cell r="C165">
-            <v>1</v>
-          </cell>
-          <cell r="D165">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="166">
-          <cell r="A166" t="str">
-            <v>on ice cold dour</v>
-          </cell>
-          <cell r="B166">
-            <v>1</v>
-          </cell>
-          <cell r="C166">
-            <v>0</v>
-          </cell>
-          <cell r="D166">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="167">
-          <cell r="A167" t="str">
-            <v>on ice call dour</v>
-          </cell>
-          <cell r="B167">
-            <v>1</v>
-          </cell>
-          <cell r="C167">
-            <v>0</v>
-          </cell>
-          <cell r="D167">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="168">
-          <cell r="A168" t="str">
-            <v>on eyes cold over</v>
-          </cell>
-          <cell r="B168">
-            <v>1</v>
-          </cell>
-          <cell r="C168">
-            <v>1</v>
-          </cell>
-          <cell r="D168">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="169">
-          <cell r="A169" t="str">
-            <v>on ice core bower</v>
-          </cell>
-          <cell r="B169">
-            <v>1</v>
-          </cell>
-          <cell r="C169">
-            <v>1</v>
-          </cell>
-          <cell r="D169">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="170">
-          <cell r="A170" t="str">
-            <v>on ice co dover</v>
-          </cell>
-          <cell r="B170">
-            <v>1</v>
-          </cell>
-          <cell r="C170">
-            <v>1</v>
-          </cell>
-          <cell r="D170">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="171">
-          <cell r="A171" t="str">
-            <v>on ice cold our</v>
-          </cell>
-          <cell r="B171">
-            <v>1</v>
-          </cell>
-          <cell r="C171">
-            <v>0</v>
-          </cell>
-          <cell r="D171">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="172">
-          <cell r="A172" t="str">
-            <v>a nice pollard</v>
-          </cell>
-          <cell r="B172">
-            <v>1</v>
-          </cell>
-          <cell r="C172">
-            <v>1</v>
-          </cell>
-          <cell r="D172">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="173">
-          <cell r="A173" t="str">
-            <v>all eyes cold hour</v>
-          </cell>
-          <cell r="B173">
-            <v>1</v>
-          </cell>
-          <cell r="C173">
-            <v>0</v>
-          </cell>
-          <cell r="D173">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="174">
-          <cell r="A174" t="str">
-            <v>on a nice cold hour</v>
-          </cell>
-          <cell r="B174">
-            <v>1</v>
-          </cell>
-          <cell r="C174">
-            <v>0</v>
-          </cell>
-          <cell r="D174">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="175">
-          <cell r="A175" t="str">
-            <v>on ice cold air</v>
-          </cell>
-          <cell r="B175">
-            <v>1</v>
-          </cell>
-          <cell r="C175">
-            <v>0</v>
-          </cell>
-          <cell r="D175">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="176">
-          <cell r="A176" t="str">
-            <v>on iced cold hour</v>
-          </cell>
-          <cell r="B176">
-            <v>1</v>
-          </cell>
-          <cell r="C176">
-            <v>0</v>
-          </cell>
-          <cell r="D176">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="177">
-          <cell r="A177" t="str">
-            <v>on eis kol dour</v>
-          </cell>
-          <cell r="B177">
-            <v>1</v>
-          </cell>
-          <cell r="C177">
-            <v>0</v>
-          </cell>
-          <cell r="D177">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
@@ -32873,6 +30412,7 @@
       <sheetData sheetId="11"/>
       <sheetData sheetId="12"/>
       <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -51914,7 +49454,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>